<commit_message>
modified list and form
</commit_message>
<xml_diff>
--- a/Applications/PSAMemberslist.xlsx
+++ b/Applications/PSAMemberslist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\psa-constitution\Applications\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6919568F-04AF-4059-9B02-D9D36EEBD8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB04C682-23D4-4F66-8C73-93E44F7A732E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="120">
   <si>
     <t>Name</t>
   </si>
@@ -353,6 +353,36 @@
   </si>
   <si>
     <t>KIT Students</t>
+  </si>
+  <si>
+    <t>Moaz Rauf Nizami</t>
+  </si>
+  <si>
+    <t>Ulm/karlsruhe</t>
+  </si>
+  <si>
+    <t>Arslan Tahir</t>
+  </si>
+  <si>
+    <t>TUM</t>
+  </si>
+  <si>
+    <t>Civil</t>
+  </si>
+  <si>
+    <t>Arshad kazmi</t>
+  </si>
+  <si>
+    <t>Duisberg</t>
+  </si>
+  <si>
+    <t>Rastatt</t>
+  </si>
+  <si>
+    <t>Asad</t>
+  </si>
+  <si>
+    <t>Political Science</t>
   </si>
 </sst>
 </file>
@@ -735,8 +765,8 @@
   </sheetPr>
   <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1482,35 +1512,35 @@
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C42" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>108</v>
+      <c r="B43" s="7" t="s">
+        <v>79</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="9" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1518,23 +1548,47 @@
         <v>43</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="D44" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="E44" s="9" t="s">
-        <v>8</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>44</v>
       </c>
+      <c r="B45" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1649,82 +1703,95 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" s="10">
+        <f>COUNTIF(C2:C65, "*KIT*")</f>
+        <v>37</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="E66" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -1816,7 +1883,7 @@
         <v>105</v>
       </c>
       <c r="E96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1966,10 +2033,34 @@
       <c r="A108" s="1">
         <v>10</v>
       </c>
+      <c r="B108" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F108" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="109" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>11</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="110" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>